<commit_message>
updated models for release
</commit_message>
<xml_diff>
--- a/inputfile.xlsx
+++ b/inputfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\PhD\Codes\Github\PAL\Examples\wfc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279557ED-78A4-4D3A-A460-47E9619CB30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892FBB42-37C1-4556-B51D-D9E474AB2F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="-1725" windowWidth="14400" windowHeight="17400" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main Folders" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="168">
   <si>
     <t>KeyName</t>
   </si>
@@ -311,6 +311,9 @@
     <t>Comment</t>
   </si>
   <si>
+    <t>./Examples/wfc/ITFC_wfc_sample1.mat</t>
+  </si>
+  <si>
     <t>modelTag</t>
   </si>
   <si>
@@ -473,646 +476,7 @@
     <t>test_ITFC_filename</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>appTag</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>FAST_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>SLOW_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>CTRL_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>out_filename</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>output_path_in_PLC</t>
-  </si>
-  <si>
-    <t>/usbBulk0/CW2/</t>
-  </si>
-  <si>
-    <t>output_file_duration_s</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>modelTag</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slmodel_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slmodel_name</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slccode_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>inflw1</t>
-  </si>
-  <si>
-    <t>inflw2</t>
-  </si>
-  <si>
-    <t>offset1</t>
-  </si>
-  <si>
-    <t>offset2</t>
-  </si>
-  <si>
-    <t>offset3</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>host_apptag</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>appTag</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>Flag_Create_test_ITFC</t>
-  </si>
-  <si>
-    <t>test_ITFC_filename</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>appTag</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>FAST_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>SLOW_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>CTRL_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>out_filename</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>output_path_in_PLC</t>
-  </si>
-  <si>
-    <t>/usbBulk0/CW2/</t>
-  </si>
-  <si>
-    <t>output_file_duration_s</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>modelTag</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slmodel_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slmodel_name</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slccode_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>inflw1</t>
-  </si>
-  <si>
-    <t>inflw2</t>
-  </si>
-  <si>
-    <t>offset1</t>
-  </si>
-  <si>
-    <t>offset2</t>
-  </si>
-  <si>
-    <t>offset3</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>host_apptag</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>appTag</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>Flag_Create_test_ITFC</t>
-  </si>
-  <si>
-    <t>test_ITFC_filename</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>appTag</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>FAST_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>SLOW_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>CTRL_FREQ_RATIO</t>
-  </si>
-  <si>
-    <t>out_filename</t>
-  </si>
-  <si>
-    <t>hostwfc</t>
-  </si>
-  <si>
-    <t>output_path_in_PLC</t>
-  </si>
-  <si>
-    <t>/usbBulk0/CW2/</t>
-  </si>
-  <si>
-    <t>output_file_duration_s</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>modelTag</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slmodel_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slmodel_name</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>slccode_folder</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>INFLW_1</t>
-  </si>
-  <si>
-    <t>INFLW_2</t>
-  </si>
-  <si>
-    <t>OFFSET_1</t>
-  </si>
-  <si>
-    <t>OFFSET_2</t>
-  </si>
-  <si>
-    <t>OFFSET_3</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>TOGGLER</t>
-  </si>
-  <si>
-    <t>inflw1</t>
-  </si>
-  <si>
-    <t>inflw2</t>
-  </si>
-  <si>
-    <t>offset1</t>
-  </si>
-  <si>
-    <t>offset2</t>
-  </si>
-  <si>
-    <t>offset3</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>host_apptag</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>appTag</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>PLCApp_folder</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>refC_name</t>
-  </si>
-  <si>
-    <t>tumitfc</t>
-  </si>
-  <si>
-    <t>Flag_Generate_PLC_app</t>
-  </si>
-  <si>
-    <t>Flag_Create_test_ITFC</t>
-  </si>
-  <si>
-    <t>test_ITFC_filename</t>
-  </si>
-  <si>
-    <t>./Examples/wfc/ITFC_wfc.mat</t>
+    <t>./Examples/wfc/ITFC_wfc_sample1.mat</t>
   </si>
   <si>
     <t>Comment</t>
@@ -1170,7 +534,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1525,12 +889,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.109375" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1538,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1546,7 +910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1554,7 +918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1562,7 +926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1570,7 +934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1591,7 +955,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.48828125" bestFit="true" customWidth="true"/>
     <col min="2" max="2" width="13.7109375" bestFit="true" customWidth="true"/>
@@ -1604,181 +968,181 @@
     <col min="3" max="3" width="13.7109375" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
-        <v>308</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>315</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>322</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>329</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>336</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>343</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>350</v>
+        <v>138</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>351</v>
+        <v>139</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="2" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="0" t="s">
-        <v>309</v>
+        <v>97</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>316</v>
+        <v>104</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>323</v>
+        <v>111</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>330</v>
+        <v>118</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>337</v>
+        <v>125</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>344</v>
+        <v>132</v>
       </c>
       <c r="G2" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" s="0" t="s">
-        <v>310</v>
+        <v>98</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>317</v>
+        <v>105</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>324</v>
+        <v>112</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>331</v>
+        <v>119</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>338</v>
+        <v>126</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>345</v>
+        <v>133</v>
       </c>
       <c r="G3" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" s="0" t="s">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>318</v>
+        <v>106</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>325</v>
+        <v>113</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>332</v>
+        <v>120</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>339</v>
+        <v>127</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>346</v>
+        <v>134</v>
       </c>
       <c r="G4" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="0"/>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" s="0" t="s">
-        <v>312</v>
+        <v>100</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>319</v>
+        <v>107</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>326</v>
+        <v>114</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>333</v>
+        <v>121</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>340</v>
+        <v>128</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>347</v>
+        <v>135</v>
       </c>
       <c r="G5" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="0"/>
       <c r="I5" s="0"/>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" s="0" t="s">
-        <v>313</v>
+        <v>101</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>320</v>
+        <v>108</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>327</v>
+        <v>115</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>334</v>
+        <v>122</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>341</v>
+        <v>129</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>348</v>
+        <v>136</v>
       </c>
       <c r="G6" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0"/>
       <c r="I6" s="0"/>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" s="0" t="s">
-        <v>314</v>
+        <v>102</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>321</v>
+        <v>109</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>328</v>
+        <v>116</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>335</v>
+        <v>123</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>342</v>
+        <v>130</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>349</v>
+        <v>137</v>
       </c>
       <c r="G7" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
@@ -1792,51 +1156,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655C75C3-8AF9-4F2C-B9A1-15AAC7A0BD6F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7.37890625" customWidth="true"/>
     <col min="2" max="2" width="13.7109375" customWidth="true"/>
     <col min="3" max="3" width="10.37890625" customWidth="true"/>
     <col min="4" max="4" width="21.48828125" customWidth="true"/>
     <col min="5" max="5" width="19.6015625" customWidth="true"/>
-    <col min="6" max="6" width="17.15625" customWidth="true"/>
+    <col min="6" max="6" width="17.15625" bestFit="true" customWidth="true"/>
     <col min="7" max="7" width="9.48828125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
-        <v>353</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>355</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>357</v>
+        <v>145</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>359</v>
+        <v>147</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>360</v>
+        <v>148</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>361</v>
+        <v>149</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="2" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="0" t="s">
-        <v>354</v>
+        <v>142</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>356</v>
+        <v>144</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>358</v>
+        <v>146</v>
       </c>
       <c r="D2" s="0" t="b">
         <v>1</v>
@@ -1845,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>362</v>
+        <v>150</v>
       </c>
       <c r="G2" s="0"/>
     </row>
@@ -1858,11 +1224,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9DDFDF-5339-43FF-B7BC-E2F362B076EE}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7.37890625" customWidth="true"/>
     <col min="2" max="2" width="13.7109375" customWidth="true"/>
@@ -1877,53 +1243,53 @@
     <col min="11" max="11" width="9.48828125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
-        <v>364</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>366</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>368</v>
+        <v>156</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>370</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>371</v>
+        <v>159</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>372</v>
+        <v>160</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>373</v>
+        <v>161</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>374</v>
+        <v>162</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>376</v>
+        <v>164</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>378</v>
+        <v>166</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="2" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="0" t="s">
-        <v>365</v>
+        <v>153</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>367</v>
+        <v>155</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>369</v>
+        <v>157</v>
       </c>
       <c r="D2" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0">
         <v>1</v>
@@ -1935,10 +1301,10 @@
         <v>10</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>375</v>
+        <v>163</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>377</v>
+        <v>165</v>
       </c>
       <c r="J2" s="0">
         <v>60</v>
@@ -1956,12 +1322,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +1338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1980,7 +1346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1988,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1996,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2004,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2012,7 +1378,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2020,7 +1386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8" t="s">
         <v>19</v>
       </c>

</xml_diff>